<commit_message>
add perimeter to UI
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vibot\aorta-compliance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F25767-771B-4303-81AA-DA272D95B211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB18BD7-0617-48A7-A330-77925C9BBD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1350" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26136" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="298">
   <si>
     <t>loss</t>
   </si>
@@ -1111,6 +1111,105 @@
   </si>
   <si>
     <t>97.91% (+/- 1.70%)</t>
+  </si>
+  <si>
+    <t>6480 - noisy_waves</t>
+  </si>
+  <si>
+    <t>loss  0.04% (+/- 0.14%)</t>
+  </si>
+  <si>
+    <t>dice_coef  95.88% (+/- 14.00%)</t>
+  </si>
+  <si>
+    <t>iou  94.03% (+/- 14.54%)</t>
+  </si>
+  <si>
+    <t>hausdorff  6.16 (+/- 6.05)</t>
+  </si>
+  <si>
+    <t>precision  95.95% (+/- 14.65%)</t>
+  </si>
+  <si>
+    <t>recall  96.05% (+/- 12.61%)</t>
+  </si>
+  <si>
+    <t>loss  0.02% (+/- 0.02%)</t>
+  </si>
+  <si>
+    <t>97.64% (+/- 1.61%)</t>
+  </si>
+  <si>
+    <t>95.43% (+/- 2.85%)</t>
+  </si>
+  <si>
+    <t>5.66 (+/- 2.01)</t>
+  </si>
+  <si>
+    <t>98.62% (+/- 1.15%)</t>
+  </si>
+  <si>
+    <t>96.83% (+/- 3.01%)</t>
+  </si>
+  <si>
+    <t>att_res_unet-diana_healthy_marfan-lr_0.001-batch_2-augmented-instance_normalization-polygon2mask-Kfield/3</t>
+  </si>
+  <si>
+    <t>att_res_unet-diana_healthy_marfan-lr_0.001-batch_2-augmented-instance_normalization-polygon2mask-Kfield/4</t>
+  </si>
+  <si>
+    <t>att_unet-diana_healthy_marfan-lr_0.001-batch_2-augmented-instance_normalization-polygon2mask-Kfield/3</t>
+  </si>
+  <si>
+    <t>att_unet-diana_healthy_marfan-lr_0.001-batch_2-augmented-instance_normalization-polygon2mask-Kfield/4</t>
+  </si>
+  <si>
+    <t>74.13% (+/- 15.17%)</t>
+  </si>
+  <si>
+    <t>60.94% (+/- 17.19%)</t>
+  </si>
+  <si>
+    <t>16.78 (+/- 7.57)</t>
+  </si>
+  <si>
+    <t>80.38% (+/- 16.93%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 81.63% (+/- 17.35%)</t>
+  </si>
+  <si>
+    <t>loss  0.02% (+/- 0.01%)</t>
+  </si>
+  <si>
+    <t>dice_coef  97.95% (+/- 0.76%)</t>
+  </si>
+  <si>
+    <t>iou  96.00% (+/- 1.44%)</t>
+  </si>
+  <si>
+    <t>hausdorff  5.28 (+/- 1.70)</t>
+  </si>
+  <si>
+    <t>precision_1  98.12% (+/- 1.47%)</t>
+  </si>
+  <si>
+    <t>recall_1  97.87% (+/- 1.39%)</t>
+  </si>
+  <si>
+    <t>97.99% (+/- 1.64%)</t>
+  </si>
+  <si>
+    <t>98.03% (+/- 0.78%)</t>
+  </si>
+  <si>
+    <t>96.14% (+/- 1.47%)</t>
+  </si>
+  <si>
+    <t>5.24 (+/- 1.72)</t>
+  </si>
+  <si>
+    <t>98.14% (+/- 1.27%)</t>
   </si>
 </sst>
 </file>
@@ -1579,16 +1678,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90:G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="86.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="91.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.90625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.81640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="21.54296875" style="10" customWidth="1"/>
@@ -2741,6 +2840,118 @@
         <v>238</v>
       </c>
     </row>
+    <row r="81" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B87" t="s">
+        <v>266</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F87" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>